<commit_message>
Modifications for Data Preparation
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/Economic_Uncertainty/EPU_CHN.xlsx
+++ b/Data_Sources_and_Preparation/Economic_Uncertainty/EPU_CHN.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Date</t>
+    <t>EPU_CHN</t>
   </si>
   <si>
-    <t>EPU_CHN</t>
+    <t>Date</t>
   </si>
   <si>
     <t>EPU_CHN-1</t>
@@ -423,18 +423,18 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
+        <v>192.9119110107422</v>
+      </c>
+      <c r="B2">
         <v>199501</v>
-      </c>
-      <c r="B2">
-        <v>192.9119110107422</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
+        <v>193.9878540039062</v>
+      </c>
+      <c r="B3">
         <v>199502</v>
-      </c>
-      <c r="B3">
-        <v>193.9878540039062</v>
       </c>
       <c r="C3">
         <v>192.9119110107422</v>
@@ -442,10 +442,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
+        <v>88.22703552246094</v>
+      </c>
+      <c r="B4">
         <v>199503</v>
-      </c>
-      <c r="B4">
-        <v>88.22703552246094</v>
       </c>
       <c r="C4">
         <v>193.9878540039062</v>
@@ -456,10 +456,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
+        <v>131.0347137451172</v>
+      </c>
+      <c r="B5">
         <v>199504</v>
-      </c>
-      <c r="B5">
-        <v>131.0347137451172</v>
       </c>
       <c r="C5">
         <v>88.22703552246094</v>
@@ -473,10 +473,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
+        <v>177.0968627929688</v>
+      </c>
+      <c r="B6">
         <v>199505</v>
-      </c>
-      <c r="B6">
-        <v>177.0968627929688</v>
       </c>
       <c r="C6">
         <v>131.0347137451172</v>
@@ -490,10 +490,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
+        <v>79.09623718261719</v>
+      </c>
+      <c r="B7">
         <v>199506</v>
-      </c>
-      <c r="B7">
-        <v>79.09623718261719</v>
       </c>
       <c r="C7">
         <v>177.0968627929688</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
+        <v>61.73268890380859</v>
+      </c>
+      <c r="B8">
         <v>199507</v>
-      </c>
-      <c r="B8">
-        <v>61.73268890380859</v>
       </c>
       <c r="C8">
         <v>79.09623718261719</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
+        <v>52.98312377929688</v>
+      </c>
+      <c r="B9">
         <v>199508</v>
-      </c>
-      <c r="B9">
-        <v>52.98312377929688</v>
       </c>
       <c r="C9">
         <v>61.73268890380859</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
+        <v>76.82008361816406</v>
+      </c>
+      <c r="B10">
         <v>199509</v>
-      </c>
-      <c r="B10">
-        <v>76.82008361816406</v>
       </c>
       <c r="C10">
         <v>52.98312377929688</v>
@@ -567,10 +567,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
+        <v>153.8712921142578</v>
+      </c>
+      <c r="B11">
         <v>199510</v>
-      </c>
-      <c r="B11">
-        <v>153.8712921142578</v>
       </c>
       <c r="C11">
         <v>76.82008361816406</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
+        <v>100.0615005493164</v>
+      </c>
+      <c r="B12">
         <v>199511</v>
-      </c>
-      <c r="B12">
-        <v>100.0615005493164</v>
       </c>
       <c r="C12">
         <v>153.8712921142578</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
+        <v>143.1166839599609</v>
+      </c>
+      <c r="B13">
         <v>199512</v>
-      </c>
-      <c r="B13">
-        <v>143.1166839599609</v>
       </c>
       <c r="C13">
         <v>100.0615005493164</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
+        <v>128.4294586181641</v>
+      </c>
+      <c r="B14">
         <v>199601</v>
-      </c>
-      <c r="B14">
-        <v>128.4294586181641</v>
       </c>
       <c r="C14">
         <v>143.1166839599609</v>
@@ -650,10 +650,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
+        <v>111.1581878662109</v>
+      </c>
+      <c r="B15">
         <v>199602</v>
-      </c>
-      <c r="B15">
-        <v>111.1581878662109</v>
       </c>
       <c r="C15">
         <v>128.4294586181641</v>
@@ -673,10 +673,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
+        <v>69.440673828125</v>
+      </c>
+      <c r="B16">
         <v>199603</v>
-      </c>
-      <c r="B16">
-        <v>69.440673828125</v>
       </c>
       <c r="C16">
         <v>111.1581878662109</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
+        <v>63.35744094848633</v>
+      </c>
+      <c r="B17">
         <v>199604</v>
-      </c>
-      <c r="B17">
-        <v>63.35744094848633</v>
       </c>
       <c r="C17">
         <v>69.440673828125</v>
@@ -719,10 +719,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
+        <v>84.17336273193359</v>
+      </c>
+      <c r="B18">
         <v>199605</v>
-      </c>
-      <c r="B18">
-        <v>84.17336273193359</v>
       </c>
       <c r="C18">
         <v>63.35744094848633</v>
@@ -742,10 +742,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
+        <v>36.83880996704102</v>
+      </c>
+      <c r="B19">
         <v>199606</v>
-      </c>
-      <c r="B19">
-        <v>36.83880996704102</v>
       </c>
       <c r="C19">
         <v>84.17336273193359</v>
@@ -765,10 +765,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
+        <v>47.68481063842773</v>
+      </c>
+      <c r="B20">
         <v>199607</v>
-      </c>
-      <c r="B20">
-        <v>47.68481063842773</v>
       </c>
       <c r="C20">
         <v>36.83880996704102</v>
@@ -788,10 +788,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
+        <v>55.95354461669922</v>
+      </c>
+      <c r="B21">
         <v>199608</v>
-      </c>
-      <c r="B21">
-        <v>55.95354461669922</v>
       </c>
       <c r="C21">
         <v>47.68481063842773</v>
@@ -811,10 +811,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
+        <v>51.04103088378906</v>
+      </c>
+      <c r="B22">
         <v>199609</v>
-      </c>
-      <c r="B22">
-        <v>51.04103088378906</v>
       </c>
       <c r="C22">
         <v>55.95354461669922</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
+        <v>53.6197624206543</v>
+      </c>
+      <c r="B23">
         <v>199610</v>
-      </c>
-      <c r="B23">
-        <v>53.6197624206543</v>
       </c>
       <c r="C23">
         <v>51.04103088378906</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
+        <v>85.29986572265625</v>
+      </c>
+      <c r="B24">
         <v>199611</v>
-      </c>
-      <c r="B24">
-        <v>85.29986572265625</v>
       </c>
       <c r="C24">
         <v>53.6197624206543</v>
@@ -880,10 +880,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
+        <v>69.18518829345703</v>
+      </c>
+      <c r="B25">
         <v>199612</v>
-      </c>
-      <c r="B25">
-        <v>69.18518829345703</v>
       </c>
       <c r="C25">
         <v>85.29986572265625</v>
@@ -903,10 +903,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
+        <v>88.32370758056641</v>
+      </c>
+      <c r="B26">
         <v>199701</v>
-      </c>
-      <c r="B26">
-        <v>88.32370758056641</v>
       </c>
       <c r="C26">
         <v>69.18518829345703</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
+        <v>115.3486785888672</v>
+      </c>
+      <c r="B27">
         <v>199702</v>
-      </c>
-      <c r="B27">
-        <v>115.3486785888672</v>
       </c>
       <c r="C27">
         <v>88.32370758056641</v>
@@ -949,10 +949,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
+        <v>59.41058731079102</v>
+      </c>
+      <c r="B28">
         <v>199703</v>
-      </c>
-      <c r="B28">
-        <v>59.41058731079102</v>
       </c>
       <c r="C28">
         <v>115.3486785888672</v>
@@ -972,10 +972,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
+        <v>123.2713470458984</v>
+      </c>
+      <c r="B29">
         <v>199704</v>
-      </c>
-      <c r="B29">
-        <v>123.2713470458984</v>
       </c>
       <c r="C29">
         <v>59.41058731079102</v>
@@ -995,10 +995,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
+        <v>20.57983016967773</v>
+      </c>
+      <c r="B30">
         <v>199705</v>
-      </c>
-      <c r="B30">
-        <v>20.57983016967773</v>
       </c>
       <c r="C30">
         <v>123.2713470458984</v>
@@ -1018,10 +1018,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
+        <v>62.72386932373047</v>
+      </c>
+      <c r="B31">
         <v>199706</v>
-      </c>
-      <c r="B31">
-        <v>62.72386932373047</v>
       </c>
       <c r="C31">
         <v>20.57983016967773</v>
@@ -1041,10 +1041,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
+        <v>42.59028244018555</v>
+      </c>
+      <c r="B32">
         <v>199707</v>
-      </c>
-      <c r="B32">
-        <v>42.59028244018555</v>
       </c>
       <c r="C32">
         <v>62.72386932373047</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
+        <v>27.12608909606934</v>
+      </c>
+      <c r="B33">
         <v>199708</v>
-      </c>
-      <c r="B33">
-        <v>27.12608909606934</v>
       </c>
       <c r="C33">
         <v>42.59028244018555</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
+        <v>70.8626708984375</v>
+      </c>
+      <c r="B34">
         <v>199709</v>
-      </c>
-      <c r="B34">
-        <v>70.8626708984375</v>
       </c>
       <c r="C34">
         <v>27.12608909606934</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
+        <v>83.15766143798828</v>
+      </c>
+      <c r="B35">
         <v>199710</v>
-      </c>
-      <c r="B35">
-        <v>83.15766143798828</v>
       </c>
       <c r="C35">
         <v>70.8626708984375</v>
@@ -1133,10 +1133,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
+        <v>69.05574798583984</v>
+      </c>
+      <c r="B36">
         <v>199711</v>
-      </c>
-      <c r="B36">
-        <v>69.05574798583984</v>
       </c>
       <c r="C36">
         <v>83.15766143798828</v>
@@ -1156,10 +1156,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
+        <v>20.72246932983398</v>
+      </c>
+      <c r="B37">
         <v>199712</v>
-      </c>
-      <c r="B37">
-        <v>20.72246932983398</v>
       </c>
       <c r="C37">
         <v>69.05574798583984</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
+        <v>77.70583343505859</v>
+      </c>
+      <c r="B38">
         <v>199801</v>
-      </c>
-      <c r="B38">
-        <v>77.70583343505859</v>
       </c>
       <c r="C38">
         <v>20.72246932983398</v>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
+        <v>98.68479919433594</v>
+      </c>
+      <c r="B39">
         <v>199802</v>
-      </c>
-      <c r="B39">
-        <v>98.68479919433594</v>
       </c>
       <c r="C39">
         <v>77.70583343505859</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
+        <v>64.92120361328125</v>
+      </c>
+      <c r="B40">
         <v>199803</v>
-      </c>
-      <c r="B40">
-        <v>64.92120361328125</v>
       </c>
       <c r="C40">
         <v>98.68479919433594</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
+        <v>19.43977737426758</v>
+      </c>
+      <c r="B41">
         <v>199804</v>
-      </c>
-      <c r="B41">
-        <v>19.43977737426758</v>
       </c>
       <c r="C41">
         <v>64.92120361328125</v>
@@ -1271,10 +1271,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
+        <v>41.80421829223633</v>
+      </c>
+      <c r="B42">
         <v>199805</v>
-      </c>
-      <c r="B42">
-        <v>41.80421829223633</v>
       </c>
       <c r="C42">
         <v>19.43977737426758</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
+        <v>68.29856109619141</v>
+      </c>
+      <c r="B43">
         <v>199806</v>
-      </c>
-      <c r="B43">
-        <v>68.29856109619141</v>
       </c>
       <c r="C43">
         <v>41.80421829223633</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
+        <v>100.4360504150391</v>
+      </c>
+      <c r="B44">
         <v>199807</v>
-      </c>
-      <c r="B44">
-        <v>100.4360504150391</v>
       </c>
       <c r="C44">
         <v>68.29856109619141</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
+        <v>38.22539901733398</v>
+      </c>
+      <c r="B45">
         <v>199808</v>
-      </c>
-      <c r="B45">
-        <v>38.22539901733398</v>
       </c>
       <c r="C45">
         <v>100.4360504150391</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
+        <v>74.32969665527344</v>
+      </c>
+      <c r="B46">
         <v>199809</v>
-      </c>
-      <c r="B46">
-        <v>74.32969665527344</v>
       </c>
       <c r="C46">
         <v>38.22539901733398</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
+        <v>128.1186828613281</v>
+      </c>
+      <c r="B47">
         <v>199810</v>
-      </c>
-      <c r="B47">
-        <v>128.1186828613281</v>
       </c>
       <c r="C47">
         <v>74.32969665527344</v>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
+        <v>51.11582565307617</v>
+      </c>
+      <c r="B48">
         <v>199811</v>
-      </c>
-      <c r="B48">
-        <v>51.11582565307617</v>
       </c>
       <c r="C48">
         <v>128.1186828613281</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
+        <v>69.6688232421875</v>
+      </c>
+      <c r="B49">
         <v>199812</v>
-      </c>
-      <c r="B49">
-        <v>69.6688232421875</v>
       </c>
       <c r="C49">
         <v>51.11582565307617</v>
@@ -1455,10 +1455,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
+        <v>123.6696548461914</v>
+      </c>
+      <c r="B50">
         <v>199901</v>
-      </c>
-      <c r="B50">
-        <v>123.6696548461914</v>
       </c>
       <c r="C50">
         <v>69.6688232421875</v>
@@ -1478,10 +1478,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
+        <v>98.32405090332031</v>
+      </c>
+      <c r="B51">
         <v>199902</v>
-      </c>
-      <c r="B51">
-        <v>98.32405090332031</v>
       </c>
       <c r="C51">
         <v>123.6696548461914</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
+        <v>82.27812957763672</v>
+      </c>
+      <c r="B52">
         <v>199903</v>
-      </c>
-      <c r="B52">
-        <v>82.27812957763672</v>
       </c>
       <c r="C52">
         <v>98.32405090332031</v>
@@ -1524,10 +1524,10 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
+        <v>16.56603240966797</v>
+      </c>
+      <c r="B53">
         <v>199904</v>
-      </c>
-      <c r="B53">
-        <v>16.56603240966797</v>
       </c>
       <c r="C53">
         <v>82.27812957763672</v>
@@ -1547,10 +1547,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
+        <v>116.0393905639648</v>
+      </c>
+      <c r="B54">
         <v>199905</v>
-      </c>
-      <c r="B54">
-        <v>116.0393905639648</v>
       </c>
       <c r="C54">
         <v>16.56603240966797</v>
@@ -1570,10 +1570,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
+        <v>101.5225067138672</v>
+      </c>
+      <c r="B55">
         <v>199906</v>
-      </c>
-      <c r="B55">
-        <v>101.5225067138672</v>
       </c>
       <c r="C55">
         <v>116.0393905639648</v>
@@ -1593,10 +1593,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
+        <v>66.90920257568359</v>
+      </c>
+      <c r="B56">
         <v>199907</v>
-      </c>
-      <c r="B56">
-        <v>66.90920257568359</v>
       </c>
       <c r="C56">
         <v>101.5225067138672</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
+        <v>39.80082321166992</v>
+      </c>
+      <c r="B57">
         <v>199908</v>
-      </c>
-      <c r="B57">
-        <v>39.80082321166992</v>
       </c>
       <c r="C57">
         <v>66.90920257568359</v>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
+        <v>102.3025283813477</v>
+      </c>
+      <c r="B58">
         <v>199909</v>
-      </c>
-      <c r="B58">
-        <v>102.3025283813477</v>
       </c>
       <c r="C58">
         <v>39.80082321166992</v>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
+        <v>78.27619934082031</v>
+      </c>
+      <c r="B59">
         <v>199910</v>
-      </c>
-      <c r="B59">
-        <v>78.27619934082031</v>
       </c>
       <c r="C59">
         <v>102.3025283813477</v>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
+        <v>62.01696395874023</v>
+      </c>
+      <c r="B60">
         <v>199911</v>
-      </c>
-      <c r="B60">
-        <v>62.01696395874023</v>
       </c>
       <c r="C60">
         <v>78.27619934082031</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
+        <v>36.9937858581543</v>
+      </c>
+      <c r="B61">
         <v>199912</v>
-      </c>
-      <c r="B61">
-        <v>36.9937858581543</v>
       </c>
       <c r="C61">
         <v>62.01696395874023</v>
@@ -1731,10 +1731,10 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
+        <v>44.00444030761719</v>
+      </c>
+      <c r="B62">
         <v>200001</v>
-      </c>
-      <c r="B62">
-        <v>44.00444030761719</v>
       </c>
       <c r="C62">
         <v>36.9937858581543</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
+        <v>9.066708564758301</v>
+      </c>
+      <c r="B63">
         <v>200002</v>
-      </c>
-      <c r="B63">
-        <v>9.066708564758301</v>
       </c>
       <c r="C63">
         <v>44.00444030761719</v>
@@ -1777,10 +1777,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
+        <v>44.39913558959961</v>
+      </c>
+      <c r="B64">
         <v>200003</v>
-      </c>
-      <c r="B64">
-        <v>44.39913558959961</v>
       </c>
       <c r="C64">
         <v>9.066708564758301</v>
@@ -1800,10 +1800,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
+        <v>35.44141387939453</v>
+      </c>
+      <c r="B65">
         <v>200004</v>
-      </c>
-      <c r="B65">
-        <v>35.44141387939453</v>
       </c>
       <c r="C65">
         <v>44.39913558959961</v>
@@ -1823,10 +1823,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
+        <v>71.13580322265625</v>
+      </c>
+      <c r="B66">
         <v>200005</v>
-      </c>
-      <c r="B66">
-        <v>71.13580322265625</v>
       </c>
       <c r="C66">
         <v>35.44141387939453</v>
@@ -1846,10 +1846,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
+        <v>36.85697555541992</v>
+      </c>
+      <c r="B67">
         <v>200006</v>
-      </c>
-      <c r="B67">
-        <v>36.85697555541992</v>
       </c>
       <c r="C67">
         <v>71.13580322265625</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
+        <v>18.6074047088623</v>
+      </c>
+      <c r="B68">
         <v>200007</v>
-      </c>
-      <c r="B68">
-        <v>18.6074047088623</v>
       </c>
       <c r="C68">
         <v>36.85697555541992</v>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
+        <v>27.14086532592773</v>
+      </c>
+      <c r="B69">
         <v>200008</v>
-      </c>
-      <c r="B69">
-        <v>27.14086532592773</v>
       </c>
       <c r="C69">
         <v>18.6074047088623</v>
@@ -1915,10 +1915,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
+        <v>58.01004791259766</v>
+      </c>
+      <c r="B70">
         <v>200009</v>
-      </c>
-      <c r="B70">
-        <v>58.01004791259766</v>
       </c>
       <c r="C70">
         <v>27.14086532592773</v>
@@ -1938,10 +1938,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
+        <v>70.60662841796875</v>
+      </c>
+      <c r="B71">
         <v>200010</v>
-      </c>
-      <c r="B71">
-        <v>70.60662841796875</v>
       </c>
       <c r="C71">
         <v>58.01004791259766</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
+        <v>140.3679656982422</v>
+      </c>
+      <c r="B72">
         <v>200011</v>
-      </c>
-      <c r="B72">
-        <v>140.3679656982422</v>
       </c>
       <c r="C72">
         <v>70.60662841796875</v>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
+        <v>112.6115951538086</v>
+      </c>
+      <c r="B73">
         <v>200012</v>
-      </c>
-      <c r="B73">
-        <v>112.6115951538086</v>
       </c>
       <c r="C73">
         <v>140.3679656982422</v>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
+        <v>97.32544708251953</v>
+      </c>
+      <c r="B74">
         <v>200101</v>
-      </c>
-      <c r="B74">
-        <v>97.32544708251953</v>
       </c>
       <c r="C74">
         <v>112.6115951538086</v>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
+        <v>65.15024566650391</v>
+      </c>
+      <c r="B75">
         <v>200102</v>
-      </c>
-      <c r="B75">
-        <v>65.15024566650391</v>
       </c>
       <c r="C75">
         <v>97.32544708251953</v>
@@ -2053,10 +2053,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
+        <v>114.6284561157227</v>
+      </c>
+      <c r="B76">
         <v>200103</v>
-      </c>
-      <c r="B76">
-        <v>114.6284561157227</v>
       </c>
       <c r="C76">
         <v>65.15024566650391</v>
@@ -2076,10 +2076,10 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
+        <v>107.1836013793945</v>
+      </c>
+      <c r="B77">
         <v>200104</v>
-      </c>
-      <c r="B77">
-        <v>107.1836013793945</v>
       </c>
       <c r="C77">
         <v>114.6284561157227</v>
@@ -2099,10 +2099,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
+        <v>95.76116943359375</v>
+      </c>
+      <c r="B78">
         <v>200105</v>
-      </c>
-      <c r="B78">
-        <v>95.76116943359375</v>
       </c>
       <c r="C78">
         <v>107.1836013793945</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
+        <v>54.47955322265625</v>
+      </c>
+      <c r="B79">
         <v>200106</v>
-      </c>
-      <c r="B79">
-        <v>54.47955322265625</v>
       </c>
       <c r="C79">
         <v>95.76116943359375</v>
@@ -2145,10 +2145,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
+        <v>118.1753997802734</v>
+      </c>
+      <c r="B80">
         <v>200107</v>
-      </c>
-      <c r="B80">
-        <v>118.1753997802734</v>
       </c>
       <c r="C80">
         <v>54.47955322265625</v>
@@ -2168,10 +2168,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81">
+        <v>131.4792327880859</v>
+      </c>
+      <c r="B81">
         <v>200108</v>
-      </c>
-      <c r="B81">
-        <v>131.4792327880859</v>
       </c>
       <c r="C81">
         <v>118.1753997802734</v>
@@ -2191,10 +2191,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82">
+        <v>202.8777160644531</v>
+      </c>
+      <c r="B82">
         <v>200109</v>
-      </c>
-      <c r="B82">
-        <v>202.8777160644531</v>
       </c>
       <c r="C82">
         <v>131.4792327880859</v>
@@ -2214,10 +2214,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83">
+        <v>297.2353515625</v>
+      </c>
+      <c r="B83">
         <v>200110</v>
-      </c>
-      <c r="B83">
-        <v>297.2353515625</v>
       </c>
       <c r="C83">
         <v>202.8777160644531</v>
@@ -2237,10 +2237,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84">
+        <v>128.7835083007812</v>
+      </c>
+      <c r="B84">
         <v>200111</v>
-      </c>
-      <c r="B84">
-        <v>128.7835083007812</v>
       </c>
       <c r="C84">
         <v>297.2353515625</v>
@@ -2260,10 +2260,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85">
+        <v>136.8471984863281</v>
+      </c>
+      <c r="B85">
         <v>200112</v>
-      </c>
-      <c r="B85">
-        <v>136.8471984863281</v>
       </c>
       <c r="C85">
         <v>128.7835083007812</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86">
+        <v>159.8944396972656</v>
+      </c>
+      <c r="B86">
         <v>200201</v>
-      </c>
-      <c r="B86">
-        <v>159.8944396972656</v>
       </c>
       <c r="C86">
         <v>136.8471984863281</v>
@@ -2306,10 +2306,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87">
+        <v>163.7011566162109</v>
+      </c>
+      <c r="B87">
         <v>200202</v>
-      </c>
-      <c r="B87">
-        <v>163.7011566162109</v>
       </c>
       <c r="C87">
         <v>159.8944396972656</v>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88">
+        <v>140.2053527832031</v>
+      </c>
+      <c r="B88">
         <v>200203</v>
-      </c>
-      <c r="B88">
-        <v>140.2053527832031</v>
       </c>
       <c r="C88">
         <v>163.7011566162109</v>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89">
+        <v>117.485481262207</v>
+      </c>
+      <c r="B89">
         <v>200204</v>
-      </c>
-      <c r="B89">
-        <v>117.485481262207</v>
       </c>
       <c r="C89">
         <v>140.2053527832031</v>
@@ -2375,10 +2375,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90">
+        <v>33.76058959960938</v>
+      </c>
+      <c r="B90">
         <v>200205</v>
-      </c>
-      <c r="B90">
-        <v>33.76058959960938</v>
       </c>
       <c r="C90">
         <v>117.485481262207</v>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91">
+        <v>116.7775039672852</v>
+      </c>
+      <c r="B91">
         <v>200206</v>
-      </c>
-      <c r="B91">
-        <v>116.7775039672852</v>
       </c>
       <c r="C91">
         <v>33.76058959960938</v>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92">
+        <v>88.06827545166016</v>
+      </c>
+      <c r="B92">
         <v>200207</v>
-      </c>
-      <c r="B92">
-        <v>88.06827545166016</v>
       </c>
       <c r="C92">
         <v>116.7775039672852</v>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93">
+        <v>140.5309753417969</v>
+      </c>
+      <c r="B93">
         <v>200208</v>
-      </c>
-      <c r="B93">
-        <v>140.5309753417969</v>
       </c>
       <c r="C93">
         <v>88.06827545166016</v>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94">
+        <v>188.888671875</v>
+      </c>
+      <c r="B94">
         <v>200209</v>
-      </c>
-      <c r="B94">
-        <v>188.888671875</v>
       </c>
       <c r="C94">
         <v>140.5309753417969</v>
@@ -2490,10 +2490,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95">
+        <v>147.9945373535156</v>
+      </c>
+      <c r="B95">
         <v>200210</v>
-      </c>
-      <c r="B95">
-        <v>147.9945373535156</v>
       </c>
       <c r="C95">
         <v>188.888671875</v>
@@ -2513,10 +2513,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96">
+        <v>109.7590942382812</v>
+      </c>
+      <c r="B96">
         <v>200211</v>
-      </c>
-      <c r="B96">
-        <v>109.7590942382812</v>
       </c>
       <c r="C96">
         <v>147.9945373535156</v>
@@ -2536,10 +2536,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97">
+        <v>85.20969390869141</v>
+      </c>
+      <c r="B97">
         <v>200212</v>
-      </c>
-      <c r="B97">
-        <v>85.20969390869141</v>
       </c>
       <c r="C97">
         <v>109.7590942382812</v>
@@ -2559,10 +2559,10 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98">
+        <v>141.7656555175781</v>
+      </c>
+      <c r="B98">
         <v>200301</v>
-      </c>
-      <c r="B98">
-        <v>141.7656555175781</v>
       </c>
       <c r="C98">
         <v>85.20969390869141</v>
@@ -2582,10 +2582,10 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99">
+        <v>88.59653472900391</v>
+      </c>
+      <c r="B99">
         <v>200302</v>
-      </c>
-      <c r="B99">
-        <v>88.59653472900391</v>
       </c>
       <c r="C99">
         <v>141.7656555175781</v>
@@ -2605,10 +2605,10 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100">
+        <v>184.7860107421875</v>
+      </c>
+      <c r="B100">
         <v>200303</v>
-      </c>
-      <c r="B100">
-        <v>184.7860107421875</v>
       </c>
       <c r="C100">
         <v>88.59653472900391</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101">
+        <v>124.3101959228516</v>
+      </c>
+      <c r="B101">
         <v>200304</v>
-      </c>
-      <c r="B101">
-        <v>124.3101959228516</v>
       </c>
       <c r="C101">
         <v>184.7860107421875</v>
@@ -2651,10 +2651,10 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102">
+        <v>102.0359115600586</v>
+      </c>
+      <c r="B102">
         <v>200305</v>
-      </c>
-      <c r="B102">
-        <v>102.0359115600586</v>
       </c>
       <c r="C102">
         <v>124.3101959228516</v>
@@ -2674,10 +2674,10 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103">
+        <v>87.32002258300781</v>
+      </c>
+      <c r="B103">
         <v>200306</v>
-      </c>
-      <c r="B103">
-        <v>87.32002258300781</v>
       </c>
       <c r="C103">
         <v>102.0359115600586</v>
@@ -2697,10 +2697,10 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104">
+        <v>92.37224578857422</v>
+      </c>
+      <c r="B104">
         <v>200307</v>
-      </c>
-      <c r="B104">
-        <v>92.37224578857422</v>
       </c>
       <c r="C104">
         <v>87.32002258300781</v>
@@ -2720,10 +2720,10 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105">
+        <v>89.334228515625</v>
+      </c>
+      <c r="B105">
         <v>200308</v>
-      </c>
-      <c r="B105">
-        <v>89.334228515625</v>
       </c>
       <c r="C105">
         <v>92.37224578857422</v>
@@ -2743,10 +2743,10 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106">
+        <v>127.8212738037109</v>
+      </c>
+      <c r="B106">
         <v>200309</v>
-      </c>
-      <c r="B106">
-        <v>127.8212738037109</v>
       </c>
       <c r="C106">
         <v>89.334228515625</v>
@@ -2766,10 +2766,10 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107">
+        <v>106.5136337280273</v>
+      </c>
+      <c r="B107">
         <v>200310</v>
-      </c>
-      <c r="B107">
-        <v>106.5136337280273</v>
       </c>
       <c r="C107">
         <v>127.8212738037109</v>
@@ -2789,10 +2789,10 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108">
+        <v>37.15930557250977</v>
+      </c>
+      <c r="B108">
         <v>200311</v>
-      </c>
-      <c r="B108">
-        <v>37.15930557250977</v>
       </c>
       <c r="C108">
         <v>106.5136337280273</v>
@@ -2812,10 +2812,10 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109">
+        <v>97.13572692871094</v>
+      </c>
+      <c r="B109">
         <v>200312</v>
-      </c>
-      <c r="B109">
-        <v>97.13572692871094</v>
       </c>
       <c r="C109">
         <v>37.15930557250977</v>
@@ -2835,10 +2835,10 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110">
+        <v>101.1584014892578</v>
+      </c>
+      <c r="B110">
         <v>200401</v>
-      </c>
-      <c r="B110">
-        <v>101.1584014892578</v>
       </c>
       <c r="C110">
         <v>97.13572692871094</v>
@@ -2858,10 +2858,10 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111">
+        <v>46.90383148193359</v>
+      </c>
+      <c r="B111">
         <v>200402</v>
-      </c>
-      <c r="B111">
-        <v>46.90383148193359</v>
       </c>
       <c r="C111">
         <v>101.1584014892578</v>
@@ -2881,10 +2881,10 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112">
+        <v>85.35299682617188</v>
+      </c>
+      <c r="B112">
         <v>200403</v>
-      </c>
-      <c r="B112">
-        <v>85.35299682617188</v>
       </c>
       <c r="C112">
         <v>46.90383148193359</v>
@@ -2904,10 +2904,10 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113">
+        <v>43.16582870483398</v>
+      </c>
+      <c r="B113">
         <v>200404</v>
-      </c>
-      <c r="B113">
-        <v>43.16582870483398</v>
       </c>
       <c r="C113">
         <v>85.35299682617188</v>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114">
+        <v>137.9871978759766</v>
+      </c>
+      <c r="B114">
         <v>200405</v>
-      </c>
-      <c r="B114">
-        <v>137.9871978759766</v>
       </c>
       <c r="C114">
         <v>43.16582870483398</v>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115">
+        <v>59.12108612060547</v>
+      </c>
+      <c r="B115">
         <v>200406</v>
-      </c>
-      <c r="B115">
-        <v>59.12108612060547</v>
       </c>
       <c r="C115">
         <v>137.9871978759766</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116">
+        <v>50.48696136474609</v>
+      </c>
+      <c r="B116">
         <v>200407</v>
-      </c>
-      <c r="B116">
-        <v>50.48696136474609</v>
       </c>
       <c r="C116">
         <v>59.12108612060547</v>
@@ -2996,10 +2996,10 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117">
+        <v>88.03998565673828</v>
+      </c>
+      <c r="B117">
         <v>200408</v>
-      </c>
-      <c r="B117">
-        <v>88.03998565673828</v>
       </c>
       <c r="C117">
         <v>50.48696136474609</v>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118">
+        <v>92.03104400634766</v>
+      </c>
+      <c r="B118">
         <v>200409</v>
-      </c>
-      <c r="B118">
-        <v>92.03104400634766</v>
       </c>
       <c r="C118">
         <v>88.03998565673828</v>
@@ -3042,10 +3042,10 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119">
+        <v>107.5005187988281</v>
+      </c>
+      <c r="B119">
         <v>200410</v>
-      </c>
-      <c r="B119">
-        <v>107.5005187988281</v>
       </c>
       <c r="C119">
         <v>92.03104400634766</v>
@@ -3065,10 +3065,10 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120">
+        <v>93.99050140380859</v>
+      </c>
+      <c r="B120">
         <v>200411</v>
-      </c>
-      <c r="B120">
-        <v>93.99050140380859</v>
       </c>
       <c r="C120">
         <v>107.5005187988281</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121">
+        <v>96.87821197509766</v>
+      </c>
+      <c r="B121">
         <v>200412</v>
-      </c>
-      <c r="B121">
-        <v>96.87821197509766</v>
       </c>
       <c r="C121">
         <v>93.99050140380859</v>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122">
+        <v>75.73043823242188</v>
+      </c>
+      <c r="B122">
         <v>200501</v>
-      </c>
-      <c r="B122">
-        <v>75.73043823242188</v>
       </c>
       <c r="C122">
         <v>96.87821197509766</v>
@@ -3134,10 +3134,10 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123">
+        <v>32.59744644165039</v>
+      </c>
+      <c r="B123">
         <v>200502</v>
-      </c>
-      <c r="B123">
-        <v>32.59744644165039</v>
       </c>
       <c r="C123">
         <v>75.73043823242188</v>
@@ -3157,10 +3157,10 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124">
+        <v>99.00125122070312</v>
+      </c>
+      <c r="B124">
         <v>200503</v>
-      </c>
-      <c r="B124">
-        <v>99.00125122070312</v>
       </c>
       <c r="C124">
         <v>32.59744644165039</v>
@@ -3180,10 +3180,10 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125">
+        <v>50.36788558959961</v>
+      </c>
+      <c r="B125">
         <v>200504</v>
-      </c>
-      <c r="B125">
-        <v>50.36788558959961</v>
       </c>
       <c r="C125">
         <v>99.00125122070312</v>
@@ -3203,10 +3203,10 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126">
+        <v>105.3501663208008</v>
+      </c>
+      <c r="B126">
         <v>200505</v>
-      </c>
-      <c r="B126">
-        <v>105.3501663208008</v>
       </c>
       <c r="C126">
         <v>50.36788558959961</v>
@@ -3226,10 +3226,10 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127">
+        <v>42.97225952148438</v>
+      </c>
+      <c r="B127">
         <v>200506</v>
-      </c>
-      <c r="B127">
-        <v>42.97225952148438</v>
       </c>
       <c r="C127">
         <v>105.3501663208008</v>
@@ -3249,10 +3249,10 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128">
+        <v>35.55521011352539</v>
+      </c>
+      <c r="B128">
         <v>200507</v>
-      </c>
-      <c r="B128">
-        <v>35.55521011352539</v>
       </c>
       <c r="C128">
         <v>42.97225952148438</v>
@@ -3272,10 +3272,10 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129">
+        <v>92.99913787841797</v>
+      </c>
+      <c r="B129">
         <v>200508</v>
-      </c>
-      <c r="B129">
-        <v>92.99913787841797</v>
       </c>
       <c r="C129">
         <v>35.55521011352539</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130">
+        <v>68.26113891601562</v>
+      </c>
+      <c r="B130">
         <v>200509</v>
-      </c>
-      <c r="B130">
-        <v>68.26113891601562</v>
       </c>
       <c r="C130">
         <v>92.99913787841797</v>
@@ -3318,10 +3318,10 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131">
+        <v>32.72947692871094</v>
+      </c>
+      <c r="B131">
         <v>200510</v>
-      </c>
-      <c r="B131">
-        <v>32.72947692871094</v>
       </c>
       <c r="C131">
         <v>68.26113891601562</v>
@@ -3341,10 +3341,10 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132">
+        <v>86.75798034667969</v>
+      </c>
+      <c r="B132">
         <v>200511</v>
-      </c>
-      <c r="B132">
-        <v>86.75798034667969</v>
       </c>
       <c r="C132">
         <v>32.72947692871094</v>
@@ -3364,10 +3364,10 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133">
+        <v>57.22021102905273</v>
+      </c>
+      <c r="B133">
         <v>200512</v>
-      </c>
-      <c r="B133">
-        <v>57.22021102905273</v>
       </c>
       <c r="C133">
         <v>86.75798034667969</v>
@@ -3387,10 +3387,10 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134">
+        <v>83.60843658447266</v>
+      </c>
+      <c r="B134">
         <v>200601</v>
-      </c>
-      <c r="B134">
-        <v>83.60843658447266</v>
       </c>
       <c r="C134">
         <v>57.22021102905273</v>
@@ -3410,10 +3410,10 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135">
+        <v>64.71510314941406</v>
+      </c>
+      <c r="B135">
         <v>200602</v>
-      </c>
-      <c r="B135">
-        <v>64.71510314941406</v>
       </c>
       <c r="C135">
         <v>83.60843658447266</v>
@@ -3433,10 +3433,10 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136">
+        <v>84.22509765625</v>
+      </c>
+      <c r="B136">
         <v>200603</v>
-      </c>
-      <c r="B136">
-        <v>84.22509765625</v>
       </c>
       <c r="C136">
         <v>64.71510314941406</v>
@@ -3456,10 +3456,10 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137">
+        <v>133.5046997070312</v>
+      </c>
+      <c r="B137">
         <v>200604</v>
-      </c>
-      <c r="B137">
-        <v>133.5046997070312</v>
       </c>
       <c r="C137">
         <v>84.22509765625</v>
@@ -3479,10 +3479,10 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138">
+        <v>66.02268981933594</v>
+      </c>
+      <c r="B138">
         <v>200605</v>
-      </c>
-      <c r="B138">
-        <v>66.02268981933594</v>
       </c>
       <c r="C138">
         <v>133.5046997070312</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139">
+        <v>110.9243469238281</v>
+      </c>
+      <c r="B139">
         <v>200606</v>
-      </c>
-      <c r="B139">
-        <v>110.9243469238281</v>
       </c>
       <c r="C139">
         <v>66.02268981933594</v>
@@ -3525,10 +3525,10 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140">
+        <v>42.70708465576172</v>
+      </c>
+      <c r="B140">
         <v>200607</v>
-      </c>
-      <c r="B140">
-        <v>42.70708465576172</v>
       </c>
       <c r="C140">
         <v>110.9243469238281</v>
@@ -3548,10 +3548,10 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141">
+        <v>36.35945510864258</v>
+      </c>
+      <c r="B141">
         <v>200608</v>
-      </c>
-      <c r="B141">
-        <v>36.35945510864258</v>
       </c>
       <c r="C141">
         <v>42.70708465576172</v>
@@ -3571,10 +3571,10 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142">
+        <v>71.51866149902344</v>
+      </c>
+      <c r="B142">
         <v>200609</v>
-      </c>
-      <c r="B142">
-        <v>71.51866149902344</v>
       </c>
       <c r="C142">
         <v>36.35945510864258</v>
@@ -3594,10 +3594,10 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143">
+        <v>74.12514495849609</v>
+      </c>
+      <c r="B143">
         <v>200610</v>
-      </c>
-      <c r="B143">
-        <v>74.12514495849609</v>
       </c>
       <c r="C143">
         <v>71.51866149902344</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144">
+        <v>43.89590454101562</v>
+      </c>
+      <c r="B144">
         <v>200611</v>
-      </c>
-      <c r="B144">
-        <v>43.89590454101562</v>
       </c>
       <c r="C144">
         <v>74.12514495849609</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145">
+        <v>67.67839050292969</v>
+      </c>
+      <c r="B145">
         <v>200612</v>
-      </c>
-      <c r="B145">
-        <v>67.67839050292969</v>
       </c>
       <c r="C145">
         <v>43.89590454101562</v>
@@ -3663,10 +3663,10 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146">
+        <v>80.17083740234375</v>
+      </c>
+      <c r="B146">
         <v>200701</v>
-      </c>
-      <c r="B146">
-        <v>80.17083740234375</v>
       </c>
       <c r="C146">
         <v>67.67839050292969</v>
@@ -3686,10 +3686,10 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147">
+        <v>64.65911865234375</v>
+      </c>
+      <c r="B147">
         <v>200702</v>
-      </c>
-      <c r="B147">
-        <v>64.65911865234375</v>
       </c>
       <c r="C147">
         <v>80.17083740234375</v>
@@ -3709,10 +3709,10 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148">
+        <v>70.07432556152344</v>
+      </c>
+      <c r="B148">
         <v>200703</v>
-      </c>
-      <c r="B148">
-        <v>70.07432556152344</v>
       </c>
       <c r="C148">
         <v>64.65911865234375</v>
@@ -3732,10 +3732,10 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149">
+        <v>68.33134460449219</v>
+      </c>
+      <c r="B149">
         <v>200704</v>
-      </c>
-      <c r="B149">
-        <v>68.33134460449219</v>
       </c>
       <c r="C149">
         <v>70.07432556152344</v>
@@ -3755,10 +3755,10 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150">
+        <v>47.79152679443359</v>
+      </c>
+      <c r="B150">
         <v>200705</v>
-      </c>
-      <c r="B150">
-        <v>47.79152679443359</v>
       </c>
       <c r="C150">
         <v>68.33134460449219</v>
@@ -3778,10 +3778,10 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151">
+        <v>77.08946228027344</v>
+      </c>
+      <c r="B151">
         <v>200706</v>
-      </c>
-      <c r="B151">
-        <v>77.08946228027344</v>
       </c>
       <c r="C151">
         <v>47.79152679443359</v>
@@ -3801,10 +3801,10 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152">
+        <v>136.7205810546875</v>
+      </c>
+      <c r="B152">
         <v>200707</v>
-      </c>
-      <c r="B152">
-        <v>136.7205810546875</v>
       </c>
       <c r="C152">
         <v>77.08946228027344</v>
@@ -3824,10 +3824,10 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153">
+        <v>56.73624038696289</v>
+      </c>
+      <c r="B153">
         <v>200708</v>
-      </c>
-      <c r="B153">
-        <v>56.73624038696289</v>
       </c>
       <c r="C153">
         <v>136.7205810546875</v>
@@ -3847,10 +3847,10 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154">
+        <v>90.57120513916016</v>
+      </c>
+      <c r="B154">
         <v>200709</v>
-      </c>
-      <c r="B154">
-        <v>90.57120513916016</v>
       </c>
       <c r="C154">
         <v>56.73624038696289</v>
@@ -3870,10 +3870,10 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155">
+        <v>92.5426025390625</v>
+      </c>
+      <c r="B155">
         <v>200710</v>
-      </c>
-      <c r="B155">
-        <v>92.5426025390625</v>
       </c>
       <c r="C155">
         <v>90.57120513916016</v>
@@ -3893,10 +3893,10 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156">
+        <v>108.428466796875</v>
+      </c>
+      <c r="B156">
         <v>200711</v>
-      </c>
-      <c r="B156">
-        <v>108.428466796875</v>
       </c>
       <c r="C156">
         <v>92.5426025390625</v>
@@ -3916,10 +3916,10 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157">
+        <v>93.82692718505859</v>
+      </c>
+      <c r="B157">
         <v>200712</v>
-      </c>
-      <c r="B157">
-        <v>93.82692718505859</v>
       </c>
       <c r="C157">
         <v>108.428466796875</v>
@@ -3939,10 +3939,10 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158">
+        <v>142.8052368164062</v>
+      </c>
+      <c r="B158">
         <v>200801</v>
-      </c>
-      <c r="B158">
-        <v>142.8052368164062</v>
       </c>
       <c r="C158">
         <v>93.82692718505859</v>
@@ -3962,10 +3962,10 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159">
+        <v>157.7542724609375</v>
+      </c>
+      <c r="B159">
         <v>200802</v>
-      </c>
-      <c r="B159">
-        <v>157.7542724609375</v>
       </c>
       <c r="C159">
         <v>142.8052368164062</v>
@@ -3985,10 +3985,10 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160">
+        <v>174.01171875</v>
+      </c>
+      <c r="B160">
         <v>200803</v>
-      </c>
-      <c r="B160">
-        <v>174.01171875</v>
       </c>
       <c r="C160">
         <v>157.7542724609375</v>
@@ -4008,10 +4008,10 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161">
+        <v>145.5144958496094</v>
+      </c>
+      <c r="B161">
         <v>200804</v>
-      </c>
-      <c r="B161">
-        <v>145.5144958496094</v>
       </c>
       <c r="C161">
         <v>174.01171875</v>
@@ -4031,10 +4031,10 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162">
+        <v>100.6835784912109</v>
+      </c>
+      <c r="B162">
         <v>200805</v>
-      </c>
-      <c r="B162">
-        <v>100.6835784912109</v>
       </c>
       <c r="C162">
         <v>145.5144958496094</v>
@@ -4054,10 +4054,10 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163">
+        <v>157.0119323730469</v>
+      </c>
+      <c r="B163">
         <v>200806</v>
-      </c>
-      <c r="B163">
-        <v>157.0119323730469</v>
       </c>
       <c r="C163">
         <v>100.6835784912109</v>
@@ -4077,10 +4077,10 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164">
+        <v>152.117919921875</v>
+      </c>
+      <c r="B164">
         <v>200807</v>
-      </c>
-      <c r="B164">
-        <v>152.117919921875</v>
       </c>
       <c r="C164">
         <v>157.0119323730469</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165">
+        <v>205.6284484863281</v>
+      </c>
+      <c r="B165">
         <v>200808</v>
-      </c>
-      <c r="B165">
-        <v>205.6284484863281</v>
       </c>
       <c r="C165">
         <v>152.117919921875</v>
@@ -4123,10 +4123,10 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166">
+        <v>298.3870239257812</v>
+      </c>
+      <c r="B166">
         <v>200809</v>
-      </c>
-      <c r="B166">
-        <v>298.3870239257812</v>
       </c>
       <c r="C166">
         <v>205.6284484863281</v>
@@ -4146,10 +4146,10 @@
     </row>
     <row r="167" spans="1:7">
       <c r="A167">
+        <v>187.5682373046875</v>
+      </c>
+      <c r="B167">
         <v>200810</v>
-      </c>
-      <c r="B167">
-        <v>187.5682373046875</v>
       </c>
       <c r="C167">
         <v>298.3870239257812</v>
@@ -4169,10 +4169,10 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168">
+        <v>194.2370300292969</v>
+      </c>
+      <c r="B168">
         <v>200811</v>
-      </c>
-      <c r="B168">
-        <v>194.2370300292969</v>
       </c>
       <c r="C168">
         <v>187.5682373046875</v>
@@ -4192,10 +4192,10 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169">
+        <v>232.7663879394531</v>
+      </c>
+      <c r="B169">
         <v>200812</v>
-      </c>
-      <c r="B169">
-        <v>232.7663879394531</v>
       </c>
       <c r="C169">
         <v>194.2370300292969</v>
@@ -4215,10 +4215,10 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170">
+        <v>223.546875</v>
+      </c>
+      <c r="B170">
         <v>200901</v>
-      </c>
-      <c r="B170">
-        <v>223.546875</v>
       </c>
       <c r="C170">
         <v>232.7663879394531</v>
@@ -4238,10 +4238,10 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171">
+        <v>170.9781341552734</v>
+      </c>
+      <c r="B171">
         <v>200902</v>
-      </c>
-      <c r="B171">
-        <v>170.9781341552734</v>
       </c>
       <c r="C171">
         <v>223.546875</v>
@@ -4261,10 +4261,10 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172">
+        <v>184.4957580566406</v>
+      </c>
+      <c r="B172">
         <v>200903</v>
-      </c>
-      <c r="B172">
-        <v>184.4957580566406</v>
       </c>
       <c r="C172">
         <v>170.9781341552734</v>
@@ -4284,10 +4284,10 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173">
+        <v>152.913330078125</v>
+      </c>
+      <c r="B173">
         <v>200904</v>
-      </c>
-      <c r="B173">
-        <v>152.913330078125</v>
       </c>
       <c r="C173">
         <v>184.4957580566406</v>
@@ -4307,10 +4307,10 @@
     </row>
     <row r="174" spans="1:7">
       <c r="A174">
+        <v>91.16470336914062</v>
+      </c>
+      <c r="B174">
         <v>200905</v>
-      </c>
-      <c r="B174">
-        <v>91.16470336914062</v>
       </c>
       <c r="C174">
         <v>152.913330078125</v>
@@ -4330,10 +4330,10 @@
     </row>
     <row r="175" spans="1:7">
       <c r="A175">
+        <v>131.52880859375</v>
+      </c>
+      <c r="B175">
         <v>200906</v>
-      </c>
-      <c r="B175">
-        <v>131.52880859375</v>
       </c>
       <c r="C175">
         <v>91.16470336914062</v>
@@ -4353,10 +4353,10 @@
     </row>
     <row r="176" spans="1:7">
       <c r="A176">
+        <v>103.9319152832031</v>
+      </c>
+      <c r="B176">
         <v>200907</v>
-      </c>
-      <c r="B176">
-        <v>103.9319152832031</v>
       </c>
       <c r="C176">
         <v>131.52880859375</v>
@@ -4376,10 +4376,10 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177">
+        <v>92.43109130859375</v>
+      </c>
+      <c r="B177">
         <v>200908</v>
-      </c>
-      <c r="B177">
-        <v>92.43109130859375</v>
       </c>
       <c r="C177">
         <v>103.9319152832031</v>
@@ -4399,10 +4399,10 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178">
+        <v>160.9516448974609</v>
+      </c>
+      <c r="B178">
         <v>200909</v>
-      </c>
-      <c r="B178">
-        <v>160.9516448974609</v>
       </c>
       <c r="C178">
         <v>92.43109130859375</v>
@@ -4422,10 +4422,10 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179">
+        <v>75.7962646484375</v>
+      </c>
+      <c r="B179">
         <v>200910</v>
-      </c>
-      <c r="B179">
-        <v>75.7962646484375</v>
       </c>
       <c r="C179">
         <v>160.9516448974609</v>
@@ -4445,10 +4445,10 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180">
+        <v>68.89027404785156</v>
+      </c>
+      <c r="B180">
         <v>200911</v>
-      </c>
-      <c r="B180">
-        <v>68.89027404785156</v>
       </c>
       <c r="C180">
         <v>75.7962646484375</v>
@@ -4468,10 +4468,10 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181">
+        <v>74.85823059082031</v>
+      </c>
+      <c r="B181">
         <v>200912</v>
-      </c>
-      <c r="B181">
-        <v>74.85823059082031</v>
       </c>
       <c r="C181">
         <v>68.89027404785156</v>
@@ -4491,10 +4491,10 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182">
+        <v>95.78208160400391</v>
+      </c>
+      <c r="B182">
         <v>201001</v>
-      </c>
-      <c r="B182">
-        <v>95.78208160400391</v>
       </c>
       <c r="C182">
         <v>74.85823059082031</v>
@@ -4514,10 +4514,10 @@
     </row>
     <row r="183" spans="1:7">
       <c r="A183">
+        <v>103.4443740844727</v>
+      </c>
+      <c r="B183">
         <v>201002</v>
-      </c>
-      <c r="B183">
-        <v>103.4443740844727</v>
       </c>
       <c r="C183">
         <v>95.78208160400391</v>
@@ -4537,10 +4537,10 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184">
+        <v>90.39569854736328</v>
+      </c>
+      <c r="B184">
         <v>201003</v>
-      </c>
-      <c r="B184">
-        <v>90.39569854736328</v>
       </c>
       <c r="C184">
         <v>103.4443740844727</v>
@@ -4560,10 +4560,10 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185">
+        <v>46.74542999267578</v>
+      </c>
+      <c r="B185">
         <v>201004</v>
-      </c>
-      <c r="B185">
-        <v>46.74542999267578</v>
       </c>
       <c r="C185">
         <v>90.39569854736328</v>
@@ -4583,10 +4583,10 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186">
+        <v>156.5486145019531</v>
+      </c>
+      <c r="B186">
         <v>201005</v>
-      </c>
-      <c r="B186">
-        <v>156.5486145019531</v>
       </c>
       <c r="C186">
         <v>46.74542999267578</v>
@@ -4606,10 +4606,10 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187">
+        <v>130.0135040283203</v>
+      </c>
+      <c r="B187">
         <v>201006</v>
-      </c>
-      <c r="B187">
-        <v>130.0135040283203</v>
       </c>
       <c r="C187">
         <v>156.5486145019531</v>
@@ -4629,10 +4629,10 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188">
+        <v>70.815673828125</v>
+      </c>
+      <c r="B188">
         <v>201007</v>
-      </c>
-      <c r="B188">
-        <v>70.815673828125</v>
       </c>
       <c r="C188">
         <v>130.0135040283203</v>
@@ -4652,10 +4652,10 @@
     </row>
     <row r="189" spans="1:7">
       <c r="A189">
+        <v>104.1029891967773</v>
+      </c>
+      <c r="B189">
         <v>201008</v>
-      </c>
-      <c r="B189">
-        <v>104.1029891967773</v>
       </c>
       <c r="C189">
         <v>70.815673828125</v>
@@ -4675,10 +4675,10 @@
     </row>
     <row r="190" spans="1:7">
       <c r="A190">
+        <v>121.5974273681641</v>
+      </c>
+      <c r="B190">
         <v>201009</v>
-      </c>
-      <c r="B190">
-        <v>121.5974273681641</v>
       </c>
       <c r="C190">
         <v>104.1029891967773</v>
@@ -4698,10 +4698,10 @@
     </row>
     <row r="191" spans="1:7">
       <c r="A191">
+        <v>74.11595916748047</v>
+      </c>
+      <c r="B191">
         <v>201010</v>
-      </c>
-      <c r="B191">
-        <v>74.11595916748047</v>
       </c>
       <c r="C191">
         <v>121.5974273681641</v>
@@ -4721,10 +4721,10 @@
     </row>
     <row r="192" spans="1:7">
       <c r="A192">
+        <v>82.42306518554688</v>
+      </c>
+      <c r="B192">
         <v>201011</v>
-      </c>
-      <c r="B192">
-        <v>82.42306518554688</v>
       </c>
       <c r="C192">
         <v>74.11595916748047</v>
@@ -4744,10 +4744,10 @@
     </row>
     <row r="193" spans="1:7">
       <c r="A193">
+        <v>110.6732406616211</v>
+      </c>
+      <c r="B193">
         <v>201012</v>
-      </c>
-      <c r="B193">
-        <v>110.6732406616211</v>
       </c>
       <c r="C193">
         <v>82.42306518554688</v>
@@ -4767,10 +4767,10 @@
     </row>
     <row r="194" spans="1:7">
       <c r="A194">
+        <v>172.6804046630859</v>
+      </c>
+      <c r="B194">
         <v>201101</v>
-      </c>
-      <c r="B194">
-        <v>172.6804046630859</v>
       </c>
       <c r="C194">
         <v>110.6732406616211</v>
@@ -4790,10 +4790,10 @@
     </row>
     <row r="195" spans="1:7">
       <c r="A195">
+        <v>46.08258056640625</v>
+      </c>
+      <c r="B195">
         <v>201102</v>
-      </c>
-      <c r="B195">
-        <v>46.08258056640625</v>
       </c>
       <c r="C195">
         <v>172.6804046630859</v>
@@ -4813,10 +4813,10 @@
     </row>
     <row r="196" spans="1:7">
       <c r="A196">
+        <v>131.2483673095703</v>
+      </c>
+      <c r="B196">
         <v>201103</v>
-      </c>
-      <c r="B196">
-        <v>131.2483673095703</v>
       </c>
       <c r="C196">
         <v>46.08258056640625</v>
@@ -4836,10 +4836,10 @@
     </row>
     <row r="197" spans="1:7">
       <c r="A197">
+        <v>153.0111389160156</v>
+      </c>
+      <c r="B197">
         <v>201104</v>
-      </c>
-      <c r="B197">
-        <v>153.0111389160156</v>
       </c>
       <c r="C197">
         <v>131.2483673095703</v>
@@ -4859,10 +4859,10 @@
     </row>
     <row r="198" spans="1:7">
       <c r="A198">
+        <v>26.14408493041992</v>
+      </c>
+      <c r="B198">
         <v>201105</v>
-      </c>
-      <c r="B198">
-        <v>26.14408493041992</v>
       </c>
       <c r="C198">
         <v>153.0111389160156</v>
@@ -4882,10 +4882,10 @@
     </row>
     <row r="199" spans="1:7">
       <c r="A199">
+        <v>39.59001159667969</v>
+      </c>
+      <c r="B199">
         <v>201106</v>
-      </c>
-      <c r="B199">
-        <v>39.59001159667969</v>
       </c>
       <c r="C199">
         <v>26.14408493041992</v>
@@ -4905,10 +4905,10 @@
     </row>
     <row r="200" spans="1:7">
       <c r="A200">
+        <v>207.3971862792969</v>
+      </c>
+      <c r="B200">
         <v>201107</v>
-      </c>
-      <c r="B200">
-        <v>207.3971862792969</v>
       </c>
       <c r="C200">
         <v>39.59001159667969</v>
@@ -4928,10 +4928,10 @@
     </row>
     <row r="201" spans="1:7">
       <c r="A201">
+        <v>186.7314758300781</v>
+      </c>
+      <c r="B201">
         <v>201108</v>
-      </c>
-      <c r="B201">
-        <v>186.7314758300781</v>
       </c>
       <c r="C201">
         <v>207.3971862792969</v>
@@ -4951,10 +4951,10 @@
     </row>
     <row r="202" spans="1:7">
       <c r="A202">
+        <v>158.0556335449219</v>
+      </c>
+      <c r="B202">
         <v>201109</v>
-      </c>
-      <c r="B202">
-        <v>158.0556335449219</v>
       </c>
       <c r="C202">
         <v>186.7314758300781</v>
@@ -4974,10 +4974,10 @@
     </row>
     <row r="203" spans="1:7">
       <c r="A203">
+        <v>238.7096099853516</v>
+      </c>
+      <c r="B203">
         <v>201110</v>
-      </c>
-      <c r="B203">
-        <v>238.7096099853516</v>
       </c>
       <c r="C203">
         <v>158.0556335449219</v>
@@ -4997,10 +4997,10 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204">
+        <v>363.5231018066406</v>
+      </c>
+      <c r="B204">
         <v>201111</v>
-      </c>
-      <c r="B204">
-        <v>363.5231018066406</v>
       </c>
       <c r="C204">
         <v>238.7096099853516</v>
@@ -5020,10 +5020,10 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205">
+        <v>324.462646484375</v>
+      </c>
+      <c r="B205">
         <v>201112</v>
-      </c>
-      <c r="B205">
-        <v>324.462646484375</v>
       </c>
       <c r="C205">
         <v>363.5231018066406</v>
@@ -5043,10 +5043,10 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206">
+        <v>298.70263671875</v>
+      </c>
+      <c r="B206">
         <v>201201</v>
-      </c>
-      <c r="B206">
-        <v>298.70263671875</v>
       </c>
       <c r="C206">
         <v>324.462646484375</v>
@@ -5066,10 +5066,10 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207">
+        <v>236.0895233154297</v>
+      </c>
+      <c r="B207">
         <v>201202</v>
-      </c>
-      <c r="B207">
-        <v>236.0895233154297</v>
       </c>
       <c r="C207">
         <v>298.70263671875</v>
@@ -5089,10 +5089,10 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208">
+        <v>242.7279968261719</v>
+      </c>
+      <c r="B208">
         <v>201203</v>
-      </c>
-      <c r="B208">
-        <v>242.7279968261719</v>
       </c>
       <c r="C208">
         <v>236.0895233154297</v>
@@ -5112,10 +5112,10 @@
     </row>
     <row r="209" spans="1:7">
       <c r="A209">
+        <v>155.8289337158203</v>
+      </c>
+      <c r="B209">
         <v>201204</v>
-      </c>
-      <c r="B209">
-        <v>155.8289337158203</v>
       </c>
       <c r="C209">
         <v>242.7279968261719</v>
@@ -5135,10 +5135,10 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210">
+        <v>216.251953125</v>
+      </c>
+      <c r="B210">
         <v>201205</v>
-      </c>
-      <c r="B210">
-        <v>216.251953125</v>
       </c>
       <c r="C210">
         <v>155.8289337158203</v>
@@ -5158,10 +5158,10 @@
     </row>
     <row r="211" spans="1:7">
       <c r="A211">
+        <v>304.552734375</v>
+      </c>
+      <c r="B211">
         <v>201206</v>
-      </c>
-      <c r="B211">
-        <v>304.552734375</v>
       </c>
       <c r="C211">
         <v>216.251953125</v>
@@ -5181,10 +5181,10 @@
     </row>
     <row r="212" spans="1:7">
       <c r="A212">
+        <v>301.5229187011719</v>
+      </c>
+      <c r="B212">
         <v>201207</v>
-      </c>
-      <c r="B212">
-        <v>301.5229187011719</v>
       </c>
       <c r="C212">
         <v>304.552734375</v>
@@ -5204,10 +5204,10 @@
     </row>
     <row r="213" spans="1:7">
       <c r="A213">
+        <v>215.3175201416016</v>
+      </c>
+      <c r="B213">
         <v>201208</v>
-      </c>
-      <c r="B213">
-        <v>215.3175201416016</v>
       </c>
       <c r="C213">
         <v>301.5229187011719</v>
@@ -5227,10 +5227,10 @@
     </row>
     <row r="214" spans="1:7">
       <c r="A214">
+        <v>161.9789886474609</v>
+      </c>
+      <c r="B214">
         <v>201209</v>
-      </c>
-      <c r="B214">
-        <v>161.9789886474609</v>
       </c>
       <c r="C214">
         <v>215.3175201416016</v>
@@ -5250,10 +5250,10 @@
     </row>
     <row r="215" spans="1:7">
       <c r="A215">
+        <v>300.7020874023438</v>
+      </c>
+      <c r="B215">
         <v>201210</v>
-      </c>
-      <c r="B215">
-        <v>300.7020874023438</v>
       </c>
       <c r="C215">
         <v>161.9789886474609</v>
@@ -5273,10 +5273,10 @@
     </row>
     <row r="216" spans="1:7">
       <c r="A216">
+        <v>306.3358459472656</v>
+      </c>
+      <c r="B216">
         <v>201211</v>
-      </c>
-      <c r="B216">
-        <v>306.3358459472656</v>
       </c>
       <c r="C216">
         <v>300.7020874023438</v>
@@ -5296,10 +5296,10 @@
     </row>
     <row r="217" spans="1:7">
       <c r="A217">
+        <v>192.7684020996094</v>
+      </c>
+      <c r="B217">
         <v>201212</v>
-      </c>
-      <c r="B217">
-        <v>192.7684020996094</v>
       </c>
       <c r="C217">
         <v>306.3358459472656</v>
@@ -5319,10 +5319,10 @@
     </row>
     <row r="218" spans="1:7">
       <c r="A218">
+        <v>208.5545196533203</v>
+      </c>
+      <c r="B218">
         <v>201301</v>
-      </c>
-      <c r="B218">
-        <v>208.5545196533203</v>
       </c>
       <c r="C218">
         <v>192.7684020996094</v>
@@ -5342,10 +5342,10 @@
     </row>
     <row r="219" spans="1:7">
       <c r="A219">
+        <v>162.2560272216797</v>
+      </c>
+      <c r="B219">
         <v>201302</v>
-      </c>
-      <c r="B219">
-        <v>162.2560272216797</v>
       </c>
       <c r="C219">
         <v>208.5545196533203</v>
@@ -5365,10 +5365,10 @@
     </row>
     <row r="220" spans="1:7">
       <c r="A220">
+        <v>83.76907348632812</v>
+      </c>
+      <c r="B220">
         <v>201303</v>
-      </c>
-      <c r="B220">
-        <v>83.76907348632812</v>
       </c>
       <c r="C220">
         <v>162.2560272216797</v>
@@ -5388,10 +5388,10 @@
     </row>
     <row r="221" spans="1:7">
       <c r="A221">
+        <v>147.9531707763672</v>
+      </c>
+      <c r="B221">
         <v>201304</v>
-      </c>
-      <c r="B221">
-        <v>147.9531707763672</v>
       </c>
       <c r="C221">
         <v>83.76907348632812</v>
@@ -5411,10 +5411,10 @@
     </row>
     <row r="222" spans="1:7">
       <c r="A222">
+        <v>82.95886993408203</v>
+      </c>
+      <c r="B222">
         <v>201305</v>
-      </c>
-      <c r="B222">
-        <v>82.95886993408203</v>
       </c>
       <c r="C222">
         <v>147.9531707763672</v>
@@ -5434,10 +5434,10 @@
     </row>
     <row r="223" spans="1:7">
       <c r="A223">
+        <v>40.40321350097656</v>
+      </c>
+      <c r="B223">
         <v>201306</v>
-      </c>
-      <c r="B223">
-        <v>40.40321350097656</v>
       </c>
       <c r="C223">
         <v>82.95886993408203</v>
@@ -5457,10 +5457,10 @@
     </row>
     <row r="224" spans="1:7">
       <c r="A224">
+        <v>115.4674758911133</v>
+      </c>
+      <c r="B224">
         <v>201307</v>
-      </c>
-      <c r="B224">
-        <v>115.4674758911133</v>
       </c>
       <c r="C224">
         <v>40.40321350097656</v>
@@ -5480,10 +5480,10 @@
     </row>
     <row r="225" spans="1:7">
       <c r="A225">
+        <v>139.7595367431641</v>
+      </c>
+      <c r="B225">
         <v>201308</v>
-      </c>
-      <c r="B225">
-        <v>139.7595367431641</v>
       </c>
       <c r="C225">
         <v>115.4674758911133</v>
@@ -5503,10 +5503,10 @@
     </row>
     <row r="226" spans="1:7">
       <c r="A226">
+        <v>69.79080200195312</v>
+      </c>
+      <c r="B226">
         <v>201309</v>
-      </c>
-      <c r="B226">
-        <v>69.79080200195312</v>
       </c>
       <c r="C226">
         <v>139.7595367431641</v>
@@ -5526,10 +5526,10 @@
     </row>
     <row r="227" spans="1:7">
       <c r="A227">
+        <v>97.59776306152344</v>
+      </c>
+      <c r="B227">
         <v>201310</v>
-      </c>
-      <c r="B227">
-        <v>97.59776306152344</v>
       </c>
       <c r="C227">
         <v>69.79080200195312</v>
@@ -5549,10 +5549,10 @@
     </row>
     <row r="228" spans="1:7">
       <c r="A228">
+        <v>81.02541351318359</v>
+      </c>
+      <c r="B228">
         <v>201311</v>
-      </c>
-      <c r="B228">
-        <v>81.02541351318359</v>
       </c>
       <c r="C228">
         <v>97.59776306152344</v>
@@ -5572,10 +5572,10 @@
     </row>
     <row r="229" spans="1:7">
       <c r="A229">
+        <v>137.2324523925781</v>
+      </c>
+      <c r="B229">
         <v>201312</v>
-      </c>
-      <c r="B229">
-        <v>137.2324523925781</v>
       </c>
       <c r="C229">
         <v>81.02541351318359</v>
@@ -5595,10 +5595,10 @@
     </row>
     <row r="230" spans="1:7">
       <c r="A230">
+        <v>103.4443740844727</v>
+      </c>
+      <c r="B230">
         <v>201401</v>
-      </c>
-      <c r="B230">
-        <v>103.4443740844727</v>
       </c>
       <c r="C230">
         <v>137.2324523925781</v>
@@ -5618,10 +5618,10 @@
     </row>
     <row r="231" spans="1:7">
       <c r="A231">
+        <v>66.52954864501953</v>
+      </c>
+      <c r="B231">
         <v>201402</v>
-      </c>
-      <c r="B231">
-        <v>66.52954864501953</v>
       </c>
       <c r="C231">
         <v>103.4443740844727</v>
@@ -5641,10 +5641,10 @@
     </row>
     <row r="232" spans="1:7">
       <c r="A232">
+        <v>134.9426116943359</v>
+      </c>
+      <c r="B232">
         <v>201403</v>
-      </c>
-      <c r="B232">
-        <v>134.9426116943359</v>
       </c>
       <c r="C232">
         <v>66.52954864501953</v>
@@ -5664,10 +5664,10 @@
     </row>
     <row r="233" spans="1:7">
       <c r="A233">
+        <v>84.26825714111328</v>
+      </c>
+      <c r="B233">
         <v>201404</v>
-      </c>
-      <c r="B233">
-        <v>84.26825714111328</v>
       </c>
       <c r="C233">
         <v>134.9426116943359</v>
@@ -5687,10 +5687,10 @@
     </row>
     <row r="234" spans="1:7">
       <c r="A234">
+        <v>80.76277160644531</v>
+      </c>
+      <c r="B234">
         <v>201405</v>
-      </c>
-      <c r="B234">
-        <v>80.76277160644531</v>
       </c>
       <c r="C234">
         <v>84.26825714111328</v>
@@ -5710,10 +5710,10 @@
     </row>
     <row r="235" spans="1:7">
       <c r="A235">
+        <v>102.2316513061523</v>
+      </c>
+      <c r="B235">
         <v>201406</v>
-      </c>
-      <c r="B235">
-        <v>102.2316513061523</v>
       </c>
       <c r="C235">
         <v>80.76277160644531</v>
@@ -5733,10 +5733,10 @@
     </row>
     <row r="236" spans="1:7">
       <c r="A236">
+        <v>127.4802856445312</v>
+      </c>
+      <c r="B236">
         <v>201407</v>
-      </c>
-      <c r="B236">
-        <v>127.4802856445312</v>
       </c>
       <c r="C236">
         <v>102.2316513061523</v>
@@ -5756,10 +5756,10 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237">
+        <v>151.0019073486328</v>
+      </c>
+      <c r="B237">
         <v>201408</v>
-      </c>
-      <c r="B237">
-        <v>151.0019073486328</v>
       </c>
       <c r="C237">
         <v>127.4802856445312</v>
@@ -5779,10 +5779,10 @@
     </row>
     <row r="238" spans="1:7">
       <c r="A238">
+        <v>185.7619018554688</v>
+      </c>
+      <c r="B238">
         <v>201409</v>
-      </c>
-      <c r="B238">
-        <v>185.7619018554688</v>
       </c>
       <c r="C238">
         <v>151.0019073486328</v>
@@ -5802,10 +5802,10 @@
     </row>
     <row r="239" spans="1:7">
       <c r="A239">
+        <v>240.4953155517578</v>
+      </c>
+      <c r="B239">
         <v>201410</v>
-      </c>
-      <c r="B239">
-        <v>240.4953155517578</v>
       </c>
       <c r="C239">
         <v>185.7619018554688</v>
@@ -5825,10 +5825,10 @@
     </row>
     <row r="240" spans="1:7">
       <c r="A240">
+        <v>112.7389831542969</v>
+      </c>
+      <c r="B240">
         <v>201411</v>
-      </c>
-      <c r="B240">
-        <v>112.7389831542969</v>
       </c>
       <c r="C240">
         <v>240.4953155517578</v>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="241" spans="1:7">
       <c r="A241">
+        <v>93.96096038818359</v>
+      </c>
+      <c r="B241">
         <v>201412</v>
-      </c>
-      <c r="B241">
-        <v>93.96096038818359</v>
       </c>
       <c r="C241">
         <v>112.7389831542969</v>
@@ -5871,10 +5871,10 @@
     </row>
     <row r="242" spans="1:7">
       <c r="A242">
+        <v>232.2151031494141</v>
+      </c>
+      <c r="B242">
         <v>201501</v>
-      </c>
-      <c r="B242">
-        <v>232.2151031494141</v>
       </c>
       <c r="C242">
         <v>93.96096038818359</v>
@@ -5894,10 +5894,10 @@
     </row>
     <row r="243" spans="1:7">
       <c r="A243">
+        <v>117.6836700439453</v>
+      </c>
+      <c r="B243">
         <v>201502</v>
-      </c>
-      <c r="B243">
-        <v>117.6836700439453</v>
       </c>
       <c r="C243">
         <v>232.2151031494141</v>
@@ -5917,10 +5917,10 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244">
+        <v>82.09329223632812</v>
+      </c>
+      <c r="B244">
         <v>201503</v>
-      </c>
-      <c r="B244">
-        <v>82.09329223632812</v>
       </c>
       <c r="C244">
         <v>117.6836700439453</v>
@@ -5940,10 +5940,10 @@
     </row>
     <row r="245" spans="1:7">
       <c r="A245">
+        <v>105.3183517456055</v>
+      </c>
+      <c r="B245">
         <v>201504</v>
-      </c>
-      <c r="B245">
-        <v>105.3183517456055</v>
       </c>
       <c r="C245">
         <v>82.09329223632812</v>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246">
+        <v>127.5528106689453</v>
+      </c>
+      <c r="B246">
         <v>201505</v>
-      </c>
-      <c r="B246">
-        <v>127.5528106689453</v>
       </c>
       <c r="C246">
         <v>105.3183517456055</v>
@@ -5986,10 +5986,10 @@
     </row>
     <row r="247" spans="1:7">
       <c r="A247">
+        <v>123.3431396484375</v>
+      </c>
+      <c r="B247">
         <v>201506</v>
-      </c>
-      <c r="B247">
-        <v>123.3431396484375</v>
       </c>
       <c r="C247">
         <v>127.5528106689453</v>
@@ -6009,10 +6009,10 @@
     </row>
     <row r="248" spans="1:7">
       <c r="A248">
+        <v>268.7091979980469</v>
+      </c>
+      <c r="B248">
         <v>201507</v>
-      </c>
-      <c r="B248">
-        <v>268.7091979980469</v>
       </c>
       <c r="C248">
         <v>123.3431396484375</v>
@@ -6032,10 +6032,10 @@
     </row>
     <row r="249" spans="1:7">
       <c r="A249">
+        <v>224.05859375</v>
+      </c>
+      <c r="B249">
         <v>201508</v>
-      </c>
-      <c r="B249">
-        <v>224.05859375</v>
       </c>
       <c r="C249">
         <v>268.7091979980469</v>
@@ -6055,10 +6055,10 @@
     </row>
     <row r="250" spans="1:7">
       <c r="A250">
+        <v>393.2341003417969</v>
+      </c>
+      <c r="B250">
         <v>201509</v>
-      </c>
-      <c r="B250">
-        <v>393.2341003417969</v>
       </c>
       <c r="C250">
         <v>224.05859375</v>
@@ -6078,10 +6078,10 @@
     </row>
     <row r="251" spans="1:7">
       <c r="A251">
+        <v>244.8679504394531</v>
+      </c>
+      <c r="B251">
         <v>201510</v>
-      </c>
-      <c r="B251">
-        <v>244.8679504394531</v>
       </c>
       <c r="C251">
         <v>393.2341003417969</v>
@@ -6101,10 +6101,10 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252">
+        <v>104.7490768432617</v>
+      </c>
+      <c r="B252">
         <v>201511</v>
-      </c>
-      <c r="B252">
-        <v>104.7490768432617</v>
       </c>
       <c r="C252">
         <v>244.8679504394531</v>
@@ -6124,10 +6124,10 @@
     </row>
     <row r="253" spans="1:7">
       <c r="A253">
+        <v>151.6144866943359</v>
+      </c>
+      <c r="B253">
         <v>201512</v>
-      </c>
-      <c r="B253">
-        <v>151.6144866943359</v>
       </c>
       <c r="C253">
         <v>104.7490768432617</v>
@@ -6147,10 +6147,10 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254">
+        <v>261.9420776367188</v>
+      </c>
+      <c r="B254">
         <v>201601</v>
-      </c>
-      <c r="B254">
-        <v>261.9420776367188</v>
       </c>
       <c r="C254">
         <v>151.6144866943359</v>
@@ -6170,10 +6170,10 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255">
+        <v>269.0191955566406</v>
+      </c>
+      <c r="B255">
         <v>201602</v>
-      </c>
-      <c r="B255">
-        <v>269.0191955566406</v>
       </c>
       <c r="C255">
         <v>261.9420776367188</v>
@@ -6193,10 +6193,10 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256">
+        <v>323.1558532714844</v>
+      </c>
+      <c r="B256">
         <v>201603</v>
-      </c>
-      <c r="B256">
-        <v>323.1558532714844</v>
       </c>
       <c r="C256">
         <v>269.0191955566406</v>
@@ -6216,10 +6216,10 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257">
+        <v>286.1773376464844</v>
+      </c>
+      <c r="B257">
         <v>201604</v>
-      </c>
-      <c r="B257">
-        <v>286.1773376464844</v>
       </c>
       <c r="C257">
         <v>323.1558532714844</v>
@@ -6239,10 +6239,10 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258">
+        <v>260.2574768066406</v>
+      </c>
+      <c r="B258">
         <v>201605</v>
-      </c>
-      <c r="B258">
-        <v>260.2574768066406</v>
       </c>
       <c r="C258">
         <v>286.1773376464844</v>
@@ -6262,10 +6262,10 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259">
+        <v>357.2088012695312</v>
+      </c>
+      <c r="B259">
         <v>201606</v>
-      </c>
-      <c r="B259">
-        <v>357.2088012695312</v>
       </c>
       <c r="C259">
         <v>260.2574768066406</v>
@@ -6285,10 +6285,10 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260">
+        <v>558.22216796875</v>
+      </c>
+      <c r="B260">
         <v>201607</v>
-      </c>
-      <c r="B260">
-        <v>558.22216796875</v>
       </c>
       <c r="C260">
         <v>357.2088012695312</v>
@@ -6308,10 +6308,10 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261">
+        <v>288.7802124023438</v>
+      </c>
+      <c r="B261">
         <v>201608</v>
-      </c>
-      <c r="B261">
-        <v>288.7802124023438</v>
       </c>
       <c r="C261">
         <v>558.22216796875</v>
@@ -6331,10 +6331,10 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262">
+        <v>388.7496032714844</v>
+      </c>
+      <c r="B262">
         <v>201609</v>
-      </c>
-      <c r="B262">
-        <v>388.7496032714844</v>
       </c>
       <c r="C262">
         <v>288.7802124023438</v>
@@ -6354,10 +6354,10 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263">
+        <v>261.8988952636719</v>
+      </c>
+      <c r="B263">
         <v>201610</v>
-      </c>
-      <c r="B263">
-        <v>261.8988952636719</v>
       </c>
       <c r="C263">
         <v>388.7496032714844</v>
@@ -6377,10 +6377,10 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264">
+        <v>475.6709289550781</v>
+      </c>
+      <c r="B264">
         <v>201611</v>
-      </c>
-      <c r="B264">
-        <v>475.6709289550781</v>
       </c>
       <c r="C264">
         <v>261.8988952636719</v>
@@ -6400,10 +6400,10 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265">
+        <v>646.9110107421875</v>
+      </c>
+      <c r="B265">
         <v>201612</v>
-      </c>
-      <c r="B265">
-        <v>646.9110107421875</v>
       </c>
       <c r="C265">
         <v>475.6709289550781</v>
@@ -6423,10 +6423,10 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266">
+        <v>694.8494262695312</v>
+      </c>
+      <c r="B266">
         <v>201701</v>
-      </c>
-      <c r="B266">
-        <v>694.8494262695312</v>
       </c>
       <c r="C266">
         <v>646.9110107421875</v>
@@ -6446,10 +6446,10 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267">
+        <v>464.5228271484375</v>
+      </c>
+      <c r="B267">
         <v>201702</v>
-      </c>
-      <c r="B267">
-        <v>464.5228271484375</v>
       </c>
       <c r="C267">
         <v>694.8494262695312</v>
@@ -6469,10 +6469,10 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268">
+        <v>533.3043823242188</v>
+      </c>
+      <c r="B268">
         <v>201703</v>
-      </c>
-      <c r="B268">
-        <v>533.3043823242188</v>
       </c>
       <c r="C268">
         <v>464.5228271484375</v>
@@ -6492,10 +6492,10 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269">
+        <v>322.3442687988281</v>
+      </c>
+      <c r="B269">
         <v>201704</v>
-      </c>
-      <c r="B269">
-        <v>322.3442687988281</v>
       </c>
       <c r="C269">
         <v>533.3043823242188</v>
@@ -6515,10 +6515,10 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270">
+        <v>451.978515625</v>
+      </c>
+      <c r="B270">
         <v>201705</v>
-      </c>
-      <c r="B270">
-        <v>451.978515625</v>
       </c>
       <c r="C270">
         <v>322.3442687988281</v>
@@ -6538,10 +6538,10 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271">
+        <v>328.5535888671875</v>
+      </c>
+      <c r="B271">
         <v>201706</v>
-      </c>
-      <c r="B271">
-        <v>328.5535888671875</v>
       </c>
       <c r="C271">
         <v>451.978515625</v>
@@ -6561,10 +6561,10 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272">
+        <v>162.6932830810547</v>
+      </c>
+      <c r="B272">
         <v>201707</v>
-      </c>
-      <c r="B272">
-        <v>162.6932830810547</v>
       </c>
       <c r="C272">
         <v>328.5535888671875</v>
@@ -6584,10 +6584,10 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273">
+        <v>265.2581176757812</v>
+      </c>
+      <c r="B273">
         <v>201708</v>
-      </c>
-      <c r="B273">
-        <v>265.2581176757812</v>
       </c>
       <c r="C273">
         <v>162.6932830810547</v>
@@ -6607,10 +6607,10 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274">
+        <v>314.001220703125</v>
+      </c>
+      <c r="B274">
         <v>201709</v>
-      </c>
-      <c r="B274">
-        <v>314.001220703125</v>
       </c>
       <c r="C274">
         <v>265.2581176757812</v>
@@ -6630,10 +6630,10 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275">
+        <v>291.5835876464844</v>
+      </c>
+      <c r="B275">
         <v>201710</v>
-      </c>
-      <c r="B275">
-        <v>291.5835876464844</v>
       </c>
       <c r="C275">
         <v>314.001220703125</v>
@@ -6653,10 +6653,10 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276">
+        <v>268.0438537597656</v>
+      </c>
+      <c r="B276">
         <v>201711</v>
-      </c>
-      <c r="B276">
-        <v>268.0438537597656</v>
       </c>
       <c r="C276">
         <v>291.5835876464844</v>
@@ -6676,10 +6676,10 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277">
+        <v>269.3547668457031</v>
+      </c>
+      <c r="B277">
         <v>201712</v>
-      </c>
-      <c r="B277">
-        <v>269.3547668457031</v>
       </c>
       <c r="C277">
         <v>268.0438537597656</v>
@@ -6699,10 +6699,10 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278">
+        <v>122.9374008178711</v>
+      </c>
+      <c r="B278">
         <v>201801</v>
-      </c>
-      <c r="B278">
-        <v>122.9374008178711</v>
       </c>
       <c r="C278">
         <v>269.3547668457031</v>
@@ -6722,10 +6722,10 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279">
+        <v>211.7801818847656</v>
+      </c>
+      <c r="B279">
         <v>201802</v>
-      </c>
-      <c r="B279">
-        <v>211.7801818847656</v>
       </c>
       <c r="C279">
         <v>122.9374008178711</v>
@@ -6745,10 +6745,10 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280">
+        <v>245.5517120361328</v>
+      </c>
+      <c r="B280">
         <v>201803</v>
-      </c>
-      <c r="B280">
-        <v>245.5517120361328</v>
       </c>
       <c r="C280">
         <v>211.7801818847656</v>
@@ -6768,10 +6768,10 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281">
+        <v>291.3069763183594</v>
+      </c>
+      <c r="B281">
         <v>201804</v>
-      </c>
-      <c r="B281">
-        <v>291.3069763183594</v>
       </c>
       <c r="C281">
         <v>245.5517120361328</v>
@@ -6791,10 +6791,10 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282">
+        <v>374.1038208007812</v>
+      </c>
+      <c r="B282">
         <v>201805</v>
-      </c>
-      <c r="B282">
-        <v>374.1038208007812</v>
       </c>
       <c r="C282">
         <v>291.3069763183594</v>
@@ -6814,10 +6814,10 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283">
+        <v>465.4168395996094</v>
+      </c>
+      <c r="B283">
         <v>201806</v>
-      </c>
-      <c r="B283">
-        <v>465.4168395996094</v>
       </c>
       <c r="C283">
         <v>374.1038208007812</v>
@@ -6837,10 +6837,10 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284">
+        <v>561.9995727539062</v>
+      </c>
+      <c r="B284">
         <v>201807</v>
-      </c>
-      <c r="B284">
-        <v>561.9995727539062</v>
       </c>
       <c r="C284">
         <v>465.4168395996094</v>

</xml_diff>